<commit_message>
refining benford on pe
</commit_message>
<xml_diff>
--- a/tabs/benford_anomalous_years.xlsx
+++ b/tabs/benford_anomalous_years.xlsx
@@ -453,7 +453,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S12"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -500,15 +500,6 @@
       <c r="L1" s="1" t="n"/>
       <c r="M1" s="1" t="n"/>
       <c r="N1" s="1" t="n"/>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>MARGIN</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="n"/>
-      <c r="Q1" s="1" t="n"/>
-      <c r="R1" s="1" t="n"/>
-      <c r="S1" s="1" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -555,21 +546,6 @@
       <c r="N2" s="1" t="n">
         <v>2020</v>
       </c>
-      <c r="O2" s="1" t="n">
-        <v>2004</v>
-      </c>
-      <c r="P2" s="1" t="n">
-        <v>2008</v>
-      </c>
-      <c r="Q2" s="1" t="n">
-        <v>2012</v>
-      </c>
-      <c r="R2" s="1" t="n">
-        <v>2016</v>
-      </c>
-      <c r="S2" s="1" t="n">
-        <v>2020</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -621,21 +597,6 @@
       <c r="N4" t="n">
         <v>0.3059606848446417</v>
       </c>
-      <c r="O4" t="n">
-        <v>0.2194039315155358</v>
-      </c>
-      <c r="P4" t="n">
-        <v>0.2415979708306912</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>0.2029169308814204</v>
-      </c>
-      <c r="R4" t="n">
-        <v>0.1280913126188966</v>
-      </c>
-      <c r="S4" t="n">
-        <v>0.1395053899809765</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -680,21 +641,6 @@
       <c r="N5" t="n">
         <v>0.1670894102726696</v>
       </c>
-      <c r="O5" t="n">
-        <v>0.2143310082435003</v>
-      </c>
-      <c r="P5" t="n">
-        <v>0.2098922003804692</v>
-      </c>
-      <c r="Q5" t="n">
-        <v>0.1832593532022828</v>
-      </c>
-      <c r="R5" t="n">
-        <v>0.1452124286620165</v>
-      </c>
-      <c r="S5" t="n">
-        <v>0.1357006975269499</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -739,21 +685,6 @@
       <c r="N6" t="n">
         <v>0.1081166772352568</v>
       </c>
-      <c r="O6" t="n">
-        <v>0.1753329105897273</v>
-      </c>
-      <c r="P6" t="n">
-        <v>0.1613823715916297</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>0.1746987951807229</v>
-      </c>
-      <c r="R6" t="n">
-        <v>0.155992390615092</v>
-      </c>
-      <c r="S6" t="n">
-        <v>0.1471147748890298</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -798,21 +729,6 @@
       <c r="N7" t="n">
         <v>0.1005072923272036</v>
       </c>
-      <c r="O7" t="n">
-        <v>0.1391883322764743</v>
-      </c>
-      <c r="P7" t="n">
-        <v>0.1334812935954344</v>
-      </c>
-      <c r="Q7" t="n">
-        <v>0.155992390615092</v>
-      </c>
-      <c r="R7" t="n">
-        <v>0.1718452758402029</v>
-      </c>
-      <c r="S7" t="n">
-        <v>0.163284717818643</v>
-      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -857,21 +773,6 @@
       <c r="N8" t="n">
         <v>0.08148383005707038</v>
       </c>
-      <c r="O8" t="n">
-        <v>0.09987317691819911</v>
-      </c>
-      <c r="P8" t="n">
-        <v>0.09575142675967026</v>
-      </c>
-      <c r="Q8" t="n">
-        <v>0.1144578313253012</v>
-      </c>
-      <c r="R8" t="n">
-        <v>0.1807228915662651</v>
-      </c>
-      <c r="S8" t="n">
-        <v>0.1626506024096386</v>
-      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -916,21 +817,6 @@
       <c r="N9" t="n">
         <v>0.05897273303741281</v>
       </c>
-      <c r="O9" t="n">
-        <v>0.0719720989220038</v>
-      </c>
-      <c r="P9" t="n">
-        <v>0.06119213696892835</v>
-      </c>
-      <c r="Q9" t="n">
-        <v>0.07260621433100824</v>
-      </c>
-      <c r="R9" t="n">
-        <v>0.1173113506658212</v>
-      </c>
-      <c r="S9" t="n">
-        <v>0.1395053899809765</v>
-      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -975,21 +861,6 @@
       <c r="N10" t="n">
         <v>0.06119213696892835</v>
       </c>
-      <c r="O10" t="n">
-        <v>0.03329105897273304</v>
-      </c>
-      <c r="P10" t="n">
-        <v>0.03868103994927077</v>
-      </c>
-      <c r="Q10" t="n">
-        <v>0.04819277108433735</v>
-      </c>
-      <c r="R10" t="n">
-        <v>0.06467977171845275</v>
-      </c>
-      <c r="S10" t="n">
-        <v>0.07577679137603044</v>
-      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -1034,21 +905,6 @@
       <c r="N11" t="n">
         <v>0.06246036778693722</v>
       </c>
-      <c r="O11" t="n">
-        <v>0.02409638554216868</v>
-      </c>
-      <c r="P11" t="n">
-        <v>0.03329105897273304</v>
-      </c>
-      <c r="Q11" t="n">
-        <v>0.02790107799619531</v>
-      </c>
-      <c r="R11" t="n">
-        <v>0.01934051997463538</v>
-      </c>
-      <c r="S11" t="n">
-        <v>0.02251109701965758</v>
-      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -1093,28 +949,12 @@
       <c r="N12" t="n">
         <v>0.05421686746987952</v>
       </c>
-      <c r="O12" t="n">
-        <v>0.02251109701965758</v>
-      </c>
-      <c r="P12" t="n">
-        <v>0.02473050095117311</v>
-      </c>
-      <c r="Q12" t="n">
-        <v>0.01997463538363982</v>
-      </c>
-      <c r="R12" t="n">
-        <v>0.01680405833861763</v>
-      </c>
-      <c r="S12" t="n">
-        <v>0.01395053899809765</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="4">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="J1:N1"/>
     <mergeCell ref="E1:F1"/>
-    <mergeCell ref="O1:S1"/>
-    <mergeCell ref="J1:N1"/>
-    <mergeCell ref="B1:C1"/>
     <mergeCell ref="G1:I1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>